<commit_message>
Got the basic 2D platforming stuff done
Got projectiles working

Level generator in early stages
</commit_message>
<xml_diff>
--- a/DesignDocs/TOP-credits.xlsx
+++ b/DesignDocs/TOP-credits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Title Screen</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Ponyville background</t>
+  </si>
+  <si>
+    <t>littleponyforever</t>
+  </si>
+  <si>
+    <t>trixie image</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B8"/>
+  <dimension ref="A3:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +462,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Got it presentable at least
</commit_message>
<xml_diff>
--- a/DesignDocs/TOP-credits.xlsx
+++ b/DesignDocs/TOP-credits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Title Screen</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>trixie image</t>
+  </si>
+  <si>
+    <t>BronyB34r</t>
+  </si>
+  <si>
+    <t>discord image</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B9"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +476,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>